<commit_message>
updates to slides and site
</commit_message>
<xml_diff>
--- a/ENS_215/Data/Class_survey_2020.xlsx
+++ b/ENS_215/Data/Class_survey_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Major" sheetId="3" r:id="rId1"/>
@@ -567,7 +567,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,20 +587,32 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -613,7 +625,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,30 +646,48 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -670,7 +700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -686,25 +718,40 @@
       <c r="A2" t="s">
         <v>8</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -716,8 +763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="88" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +809,7 @@
         <v>22</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -778,7 +825,7 @@
         <v>24</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -882,7 +929,7 @@
         <v>37</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -890,7 +937,7 @@
         <v>38</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -954,7 +1001,7 @@
         <v>46</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -978,7 +1025,7 @@
         <v>49</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1002,7 +1049,7 @@
         <v>52</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>